<commit_message>
prototyping excel config import
</commit_message>
<xml_diff>
--- a/test/config/test_project/pipelines/tables.xlsx
+++ b/test/config/test_project/pipelines/tables.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/yetl/test/config/test_project/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF81B1CE-5490-924A-8712-DFBA71E0700B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A3327C-DAA4-1E4D-A8DE-66F2D991639C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="file_source" sheetId="2" r:id="rId1"/>
+    <sheet name="file" sheetId="3" r:id="rId2"/>
+    <sheet name="table_source" sheetId="5" r:id="rId3"/>
+    <sheet name="process_log" sheetId="4" r:id="rId4"/>
+    <sheet name="delta_lake" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
   <si>
     <t>stage</t>
   </si>
@@ -160,19 +164,175 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>partition_by</t>
+  </si>
+  <si>
+    <t>delta_constraints</t>
+  </si>
+  <si>
+    <t>z_order_by</t>
+  </si>
+  <si>
+    <t>identity</t>
+  </si>
+  <si>
+    <t>deltalake</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>container</t>
+  </si>
+  <si>
+    <t>service_account</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>directory</t>
+  </si>
+  <si>
+    <t>path_date_format</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>last_modified</t>
+  </si>
+  <si>
+    <t>last_modified_by</t>
+  </si>
+  <si>
+    <t>created_by</t>
+  </si>
+  <si>
+    <t>filename_date_format</t>
+  </si>
+  <si>
+    <t>/mnt</t>
+  </si>
+  <si>
+    <t>test_project</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>{{table}}-{{filename_date_format}}*</t>
+  </si>
+  <si>
+    <t>table_id</t>
+  </si>
+  <si>
+    <t>file_source</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>utc_time</t>
+  </si>
+  <si>
+    <t>flg</t>
+  </si>
+  <si>
+    <t>/dbx_patterns/{{table}}/{{path_date_format}}</t>
+  </si>
+  <si>
+    <t>ext</t>
+  </si>
+  <si>
+    <t>customerdetailscomplete</t>
+  </si>
+  <si>
+    <t>linked_service</t>
+  </si>
+  <si>
+    <t>compression_type</t>
+  </si>
+  <si>
+    <t>compression_level</t>
+  </si>
+  <si>
+    <t>column_delimiter</t>
+  </si>
+  <si>
+    <t>row_delimiter</t>
+  </si>
+  <si>
+    <t>encoding</t>
+  </si>
+  <si>
+    <t>escape_character</t>
+  </si>
+  <si>
+    <t>quote_character</t>
+  </si>
+  <si>
+    <t>first_row_as_header</t>
+  </si>
+  <si>
+    <t>null_value</t>
+  </si>
+  <si>
+    <t>started</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>dbo</t>
+  </si>
+  <si>
+    <t>partition</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>where</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -207,9 +367,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -218,6 +375,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,11 +696,433 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}">
-  <dimension ref="A1:S9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC54A8C-AF89-4246-97DA-43E28FFF4802}">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41AADE57-D3F0-4845-A35F-567CE9F8FC2E}">
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="7" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8124EC6A-24A7-7E49-9366-C7CE563C18F3}">
+  <dimension ref="A1:N19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J13:J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570960DA-3942-B54C-8469-254067C308A0}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}">
+  <dimension ref="A1:W17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,84 +1134,94 @@
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="16" style="1"/>
+    <col min="17" max="17" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="16" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>12</v>
+      <c r="I2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>9</v>
@@ -639,277 +1236,368 @@
         <v>12</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-    </row>
-    <row r="4" spans="1:19" s="4" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+    </row>
+    <row r="4" spans="1:23" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-    </row>
-    <row r="5" spans="1:19" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+    </row>
+    <row r="5" spans="1:23" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-    </row>
-    <row r="6" spans="1:19" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+    </row>
+    <row r="6" spans="1:23" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-    </row>
-    <row r="7" spans="1:19" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+    </row>
+    <row r="7" spans="1:23" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="6">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="5">
         <v>0.1</v>
       </c>
-      <c r="J7" s="6">
+      <c r="N7" s="5">
         <v>0</v>
       </c>
-      <c r="K7" s="6">
+      <c r="O7" s="5">
         <v>100</v>
       </c>
-      <c r="L7" s="6">
+      <c r="P7" s="5">
         <v>5</v>
       </c>
-      <c r="M7" s="6">
+      <c r="Q7" s="5">
         <v>0.2</v>
       </c>
-      <c r="N7" s="6">
+      <c r="R7" s="5">
         <v>2</v>
       </c>
-      <c r="O7" s="6">
+      <c r="S7" s="5">
         <v>1000</v>
       </c>
-      <c r="P7" s="6">
+      <c r="T7" s="5">
         <v>0</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="U7" s="5">
         <v>1</v>
       </c>
-      <c r="R7" s="6">
+      <c r="V7" s="5">
         <v>365</v>
       </c>
-      <c r="S7" s="6">
+      <c r="W7" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:23" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-    </row>
-    <row r="9" spans="1:19" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+    </row>
+    <row r="9" spans="1:23" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:L1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added unity catalog support
</commit_message>
<xml_diff>
--- a/test/config/test_project/pipelines/tables.xlsx
+++ b/test/config/test_project/pipelines/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/yetl/test/config/test_project/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C795473-8E69-E14A-8177-5CA8F0F5F1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8158DC8E-21E9-6644-930C-41088358A8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>stage</t>
   </si>
@@ -39,9 +39,6 @@
     <t>table</t>
   </si>
   <si>
-    <t>ids</t>
-  </si>
-  <si>
     <t>depends_on</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t>max_rows</t>
-  </si>
-  <si>
-    <t>mins_rows</t>
   </si>
   <si>
     <t>process_group</t>
@@ -152,9 +146,6 @@
     <t>z_order_by</t>
   </si>
   <si>
-    <t>_load_date</t>
-  </si>
-  <si>
     <t>deltalake</t>
   </si>
   <si>
@@ -171,6 +162,19 @@
   </si>
   <si>
     <t>vacuum</t>
+  </si>
+  <si>
+    <t>catalog</t>
+  </si>
+  <si>
+    <t>hive_metastore</t>
+  </si>
+  <si>
+    <t>_load_date_1
+_load_date_2</t>
+  </si>
+  <si>
+    <t>min_rows</t>
   </si>
 </sst>
 </file>
@@ -290,32 +294,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,244 +635,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="16" style="2"/>
+    <col min="3" max="3" width="19.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="3.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13" style="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="16" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:25" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="I1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="16"/>
+    </row>
+    <row r="2" spans="1:25" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="14"/>
-    </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>43</v>
-      </c>
       <c r="K2" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>46</v>
+      <c r="M2" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="N2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="R2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="X2" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="V2" s="17" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="6">
+        <v>42</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="6">
         <v>30</v>
       </c>
-      <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="7"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="13"/>
       <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
     </row>
-    <row r="4" spans="1:24" s="4" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="4" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="6">
+      <c r="M4" s="3"/>
+      <c r="N4" s="6">
         <v>30</v>
       </c>
-      <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="7"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="13"/>
       <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:24" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -876,33 +893,36 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="5"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="6"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="7"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="13"/>
       <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:24" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -910,179 +930,191 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="5"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="6"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="7"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="13"/>
       <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:24" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="6">
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="6">
         <v>30</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="6">
         <v>0.1</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <v>0</v>
       </c>
-      <c r="P7" s="6">
+      <c r="Q7" s="6">
         <v>100</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="R7" s="8">
         <v>5</v>
       </c>
-      <c r="R7" s="6">
+      <c r="S7" s="6">
         <v>0.2</v>
       </c>
-      <c r="S7" s="6">
+      <c r="T7" s="6">
         <v>2</v>
       </c>
-      <c r="T7" s="6">
+      <c r="U7" s="6">
         <v>1000</v>
       </c>
-      <c r="U7" s="6">
+      <c r="V7" s="6">
         <v>0</v>
       </c>
-      <c r="V7" s="19">
+      <c r="W7" s="14">
         <v>1</v>
       </c>
-      <c r="W7" s="6">
+      <c r="X7" s="6">
         <v>365</v>
       </c>
-      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
     </row>
-    <row r="8" spans="1:24" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="6">
+      <c r="M8" s="3"/>
+      <c r="N8" s="6">
         <v>30</v>
       </c>
-      <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="7"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="13"/>
       <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:24" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="6">
+      <c r="M9" s="3"/>
+      <c r="N9" s="6">
         <v>30</v>
       </c>
-      <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="7"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="13"/>
       <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tested unit catalog support
</commit_message>
<xml_diff>
--- a/test/config/test_project/pipelines/tables.xlsx
+++ b/test/config/test_project/pipelines/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/yetl/test/config/test_project/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8158DC8E-21E9-6644-930C-41088358A8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C510B665-4C1C-0445-9A12-05D44F1A70D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>warning_thresholds</t>
   </si>
   <si>
-    <t>error_thresholds</t>
-  </si>
-  <si>
     <t>custom_properties</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>min_rows</t>
+  </si>
+  <si>
+    <t>exception_thresholds</t>
   </si>
 </sst>
 </file>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>2</v>
@@ -687,16 +687,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
@@ -710,13 +710,13 @@
       <c r="Q1" s="18"/>
       <c r="R1" s="19"/>
       <c r="S1" s="18" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="T1" s="18"/>
       <c r="U1" s="18"/>
       <c r="V1" s="18"/>
       <c r="W1" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X1" s="16"/>
     </row>
@@ -730,86 +730,86 @@
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
       <c r="I2" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="X2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="6">
@@ -829,26 +829,26 @@
     </row>
     <row r="4" spans="1:25" s="4" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -872,19 +872,19 @@
     </row>
     <row r="5" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -909,19 +909,19 @@
     </row>
     <row r="6" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -946,33 +946,33 @@
     </row>
     <row r="7" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N7" s="6">
         <v>30</v>
@@ -1011,29 +1011,29 @@
     </row>
     <row r="8" spans="1:25" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1056,29 +1056,29 @@
     </row>
     <row r="9" spans="1:25" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>

</xml_diff>

<commit_message>
added support for delta lake liquid clustering
</commit_message>
<xml_diff>
--- a/test/config/test_project/pipelines/tables.xlsx
+++ b/test/config/test_project/pipelines/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/yetl/test/config/test_project/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C510B665-4C1C-0445-9A12-05D44F1A70D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5315BB1A-6B7C-6C42-9230-A5C087189DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>stage</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>exception_thresholds</t>
+  </si>
+  <si>
+    <t>cluster_by</t>
   </si>
 </sst>
 </file>
@@ -635,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}">
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:V1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,24 +656,25 @@
     <col min="9" max="9" width="34.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13" style="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="16" style="2"/>
+    <col min="12" max="12" width="11" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" style="2" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13" style="15" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="16" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -703,24 +707,25 @@
       <c r="L1" s="20"/>
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="20"/>
+      <c r="P1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="18" t="s">
+      <c r="R1" s="18"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="18"/>
       <c r="U1" s="18"/>
       <c r="V1" s="18"/>
-      <c r="W1" s="16" t="s">
+      <c r="W1" s="18"/>
+      <c r="X1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
     </row>
-    <row r="2" spans="1:25" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -739,46 +744,49 @@
         <v>39</v>
       </c>
       <c r="L2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="S2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="X2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -811,23 +819,26 @@
       <c r="L3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="6">
+      <c r="M3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="6">
         <v>30</v>
       </c>
-      <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="7"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="13"/>
       <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:25" s="4" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" s="4" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -855,22 +866,23 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="6">
+      <c r="N4" s="3"/>
+      <c r="O4" s="6">
         <v>30</v>
       </c>
-      <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="7"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="13"/>
       <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -894,20 +906,21 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="5"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="6"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="7"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="13"/>
       <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -931,20 +944,21 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="5"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="6"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="7"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="13"/>
       <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:25" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -971,45 +985,46 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="3"/>
+      <c r="N7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="6">
         <v>30</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <v>0.1</v>
       </c>
-      <c r="P7" s="6">
+      <c r="Q7" s="6">
         <v>0</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="R7" s="6">
         <v>100</v>
       </c>
-      <c r="R7" s="8">
+      <c r="S7" s="8">
         <v>5</v>
       </c>
-      <c r="S7" s="6">
+      <c r="T7" s="6">
         <v>0.2</v>
       </c>
-      <c r="T7" s="6">
+      <c r="U7" s="6">
         <v>2</v>
       </c>
-      <c r="U7" s="6">
+      <c r="V7" s="6">
         <v>1000</v>
       </c>
-      <c r="V7" s="6">
+      <c r="W7" s="6">
         <v>0</v>
       </c>
-      <c r="W7" s="14">
+      <c r="X7" s="14">
         <v>1</v>
       </c>
-      <c r="X7" s="6">
+      <c r="Y7" s="6">
         <v>365</v>
       </c>
-      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:25" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -1039,22 +1054,23 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="6">
+      <c r="N8" s="3"/>
+      <c r="O8" s="6">
         <v>30</v>
       </c>
-      <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="7"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="13"/>
       <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:25" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -1084,35 +1100,36 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="6">
+      <c r="N9" s="3"/>
+      <c r="O9" s="6">
         <v>30</v>
       </c>
-      <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="7"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="13"/>
       <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="X1:Y1"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:W1"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="I1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>